<commit_message>
creating Excelsheet code in genericUtils pkg
</commit_message>
<xml_diff>
--- a/ActiTime-Automation-Cucumber-Framework/resourceLib/testData/TestData.xlsx
+++ b/ActiTime-Automation-Cucumber-Framework/resourceLib/testData/TestData.xlsx
@@ -10,6 +10,7 @@
     <sheet name="LoginSheet" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -393,7 +394,7 @@
   <dimension ref="A1:S13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -716,4 +717,16 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>